<commit_message>
modifying GLDAS map data
</commit_message>
<xml_diff>
--- a/DatasetTable.xlsx
+++ b/DatasetTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yutaro\Documents\RShiny_Microclim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5A1C52-14B1-4032-8877-EFBC74FFC1F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AFED77-6553-40F6-821E-F764E1E7B9A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="39">
   <si>
     <t>Dataset</t>
   </si>
@@ -106,43 +106,37 @@
     <t>microclim</t>
   </si>
   <si>
-    <t>One day</t>
-  </si>
-  <si>
     <t>SNODAS</t>
   </si>
   <si>
     <t>NicheMapR</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>[US only, Hourly, 1991-2021, stations]</t>
-  </si>
-  <si>
-    <t>[Global, Hourly, 1981 - 2021, 0.1° x 0.1°]</t>
-  </si>
-  <si>
-    <t>[Global, 3-hourly, 2000 - 2021, 0.25° x 0.25°]</t>
-  </si>
-  <si>
-    <t>[US only, Daily, 1979 - 2021, stations]</t>
-  </si>
-  <si>
-    <t>[Global, Daily, varies by station, stations]</t>
-  </si>
-  <si>
-    <t>[Global, Hourly, 1979 - 2017, 0.6° x 0.6°]</t>
-  </si>
-  <si>
-    <t>[Global, One day, hourly for the 15th of each month, 0.17° x 0.17°]</t>
-  </si>
-  <si>
-    <t>[US only, Daily, 2003 - 2021, 0.01° x 0.01°]</t>
-  </si>
-  <si>
-    <t>[Global, Hourly, 1957 - 2021, 30m?]</t>
+    <t>SpatRes</t>
+  </si>
+  <si>
+    <t>Stations</t>
+  </si>
+  <si>
+    <t>0.1° x 0.1°</t>
+  </si>
+  <si>
+    <t>0.25° x 0.25°</t>
+  </si>
+  <si>
+    <t>0.6° x 0.6°</t>
+  </si>
+  <si>
+    <t>0.17° x 0.17°</t>
+  </si>
+  <si>
+    <t>0.01° x 0.01°</t>
+  </si>
+  <si>
+    <t>30m?</t>
+  </si>
+  <si>
+    <t>One day each month</t>
   </si>
 </sst>
 </file>
@@ -986,13 +980,13 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1006,40 +1000,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -1053,19 +1047,19 @@
         <v>2021</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -1083,10 +1077,10 @@
         <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1100,13 +1094,13 @@
         <v>2021</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
@@ -1124,16 +1118,16 @@
         <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1147,13 +1141,13 @@
         <v>2021</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -1180,7 +1174,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1194,13 +1188,13 @@
         <v>2021</v>
       </c>
       <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -1209,7 +1203,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -1218,7 +1212,7 @@
         <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -1227,7 +1221,7 @@
         <v>18</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1235,13 +1229,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -1256,19 +1250,19 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1282,13 +1276,13 @@
         <v>2017</v>
       </c>
       <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -1300,22 +1294,22 @@
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O7" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1323,13 +1317,13 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -1344,24 +1338,24 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
       </c>
       <c r="O8" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>2003</v>
@@ -1370,13 +1364,13 @@
         <v>2021</v>
       </c>
       <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -1400,15 +1394,15 @@
         <v>18</v>
       </c>
       <c r="N9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>1957</v>
@@ -1417,13 +1411,13 @@
         <v>2021</v>
       </c>
       <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
         <v>17</v>
@@ -1438,19 +1432,19 @@
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding data + spatial comparison for contUS
</commit_message>
<xml_diff>
--- a/DatasetTable.xlsx
+++ b/DatasetTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yutaro\Documents\RShiny_Microclim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AFED77-6553-40F6-821E-F764E1E7B9A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2822BA-7598-46A2-93BA-D227DEC06CBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>One day each month</t>
+  </si>
+  <si>
+    <t>0.04° x 0.04°</t>
   </si>
 </sst>
 </file>
@@ -980,7 +983,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,37 +1088,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>1981</v>
-      </c>
-      <c r="C3">
-        <v>2021</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -1132,22 +1129,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>2000</v>
+        <v>1981</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -1168,10 +1165,10 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
         <v>17</v>
@@ -1179,31 +1176,31 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>1979</v>
+        <v>2000</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -1215,27 +1212,33 @@
         <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>1979</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -1247,10 +1250,10 @@
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
         <v>17</v>
@@ -1262,7 +1265,7 @@
         <v>18</v>
       </c>
       <c r="O6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>